<commit_message>
added new logo, add admin link, and other minor changes
</commit_message>
<xml_diff>
--- a/db/seeds_databases/users_db.xlsx
+++ b/db/seeds_databases/users_db.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="340" yWindow="480" windowWidth="25600" windowHeight="15540"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="192">
   <si>
     <t>rut</t>
   </si>
@@ -597,6 +597,15 @@
   </si>
   <si>
     <t>place</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
   </si>
 </sst>
 </file>
@@ -975,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:J38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,7 +997,7 @@
     <col min="5" max="16384" width="14.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1005,19 +1014,22 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1034,17 +1046,20 @@
         <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -1061,17 +1076,20 @@
         <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -1088,17 +1106,20 @@
         <v>23</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>24</v>
       </c>
@@ -1115,17 +1136,20 @@
         <v>28</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>29</v>
       </c>
@@ -1142,19 +1166,22 @@
         <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="I6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>35</v>
       </c>
@@ -1171,19 +1198,22 @@
         <v>39</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>41</v>
       </c>
@@ -1200,17 +1230,20 @@
         <v>45</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>46</v>
       </c>
@@ -1227,19 +1260,22 @@
         <v>50</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I9" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>52</v>
       </c>
@@ -1256,17 +1292,20 @@
         <v>56</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>57</v>
       </c>
@@ -1283,17 +1322,20 @@
         <v>61</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>62</v>
       </c>
@@ -1310,17 +1352,20 @@
         <v>66</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>67</v>
       </c>
@@ -1337,17 +1382,20 @@
         <v>70</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>71</v>
       </c>
@@ -1364,17 +1412,20 @@
         <v>75</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>76</v>
       </c>
@@ -1391,17 +1442,20 @@
         <v>80</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H15" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>82</v>
       </c>
@@ -1418,19 +1472,22 @@
         <v>86</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H16" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="I16" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>88</v>
       </c>
@@ -1447,17 +1504,20 @@
         <v>92</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>93</v>
       </c>
@@ -1474,19 +1534,22 @@
         <v>97</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H18" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H18" s="2" t="s">
+      <c r="I18" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="I18" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>99</v>
       </c>
@@ -1503,19 +1566,22 @@
         <v>103</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H19" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="I19" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="I19" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>105</v>
       </c>
@@ -1532,17 +1598,20 @@
         <v>12</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>109</v>
       </c>
@@ -1559,17 +1628,20 @@
         <v>113</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>114</v>
       </c>
@@ -1586,19 +1658,22 @@
         <v>12</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="I22" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="I22" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>119</v>
       </c>
@@ -1615,19 +1690,22 @@
         <v>123</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H23" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H23" s="2" t="s">
+      <c r="I23" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="I23" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>125</v>
       </c>
@@ -1644,17 +1722,20 @@
         <v>12</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>128</v>
       </c>
@@ -1671,17 +1752,20 @@
         <v>132</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>133</v>
       </c>
@@ -1698,17 +1782,20 @@
         <v>137</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H26" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>138</v>
       </c>
@@ -1725,17 +1812,20 @@
         <v>12</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>142</v>
       </c>
@@ -1752,17 +1842,20 @@
         <v>12</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>145</v>
       </c>
@@ -1779,17 +1872,20 @@
         <v>12</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>149</v>
       </c>
@@ -1806,17 +1902,20 @@
         <v>153</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="H30" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>154</v>
       </c>
@@ -1833,19 +1932,22 @@
         <v>158</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G31" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H31" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H31" s="2" t="s">
+      <c r="I31" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="I31" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>160</v>
       </c>
@@ -1862,19 +1964,22 @@
         <v>163</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G32" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H32" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="I32" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="I32" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>165</v>
       </c>
@@ -1891,19 +1996,22 @@
         <v>169</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>13</v>
+        <v>191</v>
       </c>
       <c r="G33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="H33" s="2" t="s">
+      <c r="I33" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="I33" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>171</v>
       </c>
@@ -1920,17 +2028,20 @@
         <v>12</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>174</v>
       </c>
@@ -1947,17 +2058,20 @@
         <v>178</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2">
+        <v>13</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>12</v>
       </c>
@@ -1974,17 +2088,20 @@
         <v>12</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>183</v>
       </c>
@@ -2001,17 +2118,20 @@
         <v>12</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2">
+        <v>13</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>174</v>
       </c>
@@ -2028,12 +2148,15 @@
         <v>178</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>13</v>
+        <v>190</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="I38" s="2">
+        <v>13</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="J38" s="2">
         <v>1</v>
       </c>
     </row>

</xml_diff>